<commit_message>
corrected reference designators, added R1 and D2
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GS03FLMB_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GS03FLMB_00001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\IRAD\IRAD 2015\Programs\OOI Phase 2\Post Delivery 7 support\Asset Management Data\ingestion-csvs_20151204\ingestion-csvs\GS_mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1404" windowWidth="26016" windowHeight="15396" activeTab="1"/>
+    <workbookView xWindow="1500" yWindow="1410" windowWidth="26010" windowHeight="15390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="107">
   <si>
     <t>Ref Des</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Requires TEMPWAT, PRESWAT, and PRACSAL from GS03FLMB-RIS02-03-CTDMOG000</t>
   </si>
   <si>
-    <t>GS03FLMB-FM001-00-ENG000000</t>
-  </si>
-  <si>
     <t>54° 04.8180' S</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
     <t>P0144</t>
   </si>
   <si>
-    <t>GS03FLMB-00001-ENG</t>
-  </si>
-  <si>
     <t>[2.851669E-03,1.213603E-04,2.442175E-06,2.304734E+02,-3.134845E-01,-5.703598E+01,4.555627E+00]</t>
   </si>
   <si>
@@ -212,42 +206,6 @@
   </si>
   <si>
     <t>GS03FLMB-RIM01-02-ADCPSL007</t>
-  </si>
-  <si>
-    <t>GS03FLMB-RIM01-02-CTDMOG087</t>
-  </si>
-  <si>
-    <t>GS03FLMB-RIM01-02-CTDMOG077</t>
-  </si>
-  <si>
-    <t>GS03FLMB-RIM01-02-CTDMOG013</t>
-  </si>
-  <si>
-    <t>GS03FLMB-RIM01-02-CTDMOG012</t>
-  </si>
-  <si>
-    <t>GS03FLMB-RIM01-02-CTDMOG075</t>
-  </si>
-  <si>
-    <t>GS03FLMB-RIM01-02-CTDMOG032</t>
-  </si>
-  <si>
-    <t>GS03FLMB-RIM01-02-CTDMOG079</t>
-  </si>
-  <si>
-    <t>GS03FLMB-RIM01-02-CTDMOG031</t>
-  </si>
-  <si>
-    <t>GS03FLMB-RIM01-02-CTDMOG014</t>
-  </si>
-  <si>
-    <t>GS03FLMB-RIM01-02-CTDMOH093</t>
-  </si>
-  <si>
-    <t>GS03FLMB-RIM01-02-CTDMOH092</t>
-  </si>
-  <si>
-    <t>GS03FLMB-RIM01-02-CTDMOH084</t>
   </si>
   <si>
     <t>GS03FLMB-RIS01-04-PHSENF000</t>
@@ -368,6 +326,54 @@
   </si>
   <si>
     <t>A00959</t>
+  </si>
+  <si>
+    <t>GS03FLMB-RIM01-02-CTDMOG060</t>
+  </si>
+  <si>
+    <t>GS03FLMB-RIM01-02-CTDMOG061</t>
+  </si>
+  <si>
+    <t>GS03FLMB-RIM01-02-CTDMOG062</t>
+  </si>
+  <si>
+    <t>GS03FLMB-RIM01-02-CTDMOG063</t>
+  </si>
+  <si>
+    <t>GS03FLMB-RIM01-02-CTDMOG064</t>
+  </si>
+  <si>
+    <t>GS03FLMB-RIM01-02-CTDMOG065</t>
+  </si>
+  <si>
+    <t>GS03FLMB-RIM01-02-CTDMOG066</t>
+  </si>
+  <si>
+    <t>GS03FLMB-RIM01-02-CTDMOG067</t>
+  </si>
+  <si>
+    <t>GS03FLMB-RIM01-02-CTDMOG068</t>
+  </si>
+  <si>
+    <t>GS03FLMB-RIM01-02-CTDMOH069</t>
+  </si>
+  <si>
+    <t>GS03FLMB-RIM01-02-CTDMOH070</t>
+  </si>
+  <si>
+    <t>GS03FLMB-RIM01-02-CTDMOH071</t>
+  </si>
+  <si>
+    <t>GS03FLMB-RIM01-00-SIOENG000</t>
+  </si>
+  <si>
+    <t>GS03FLMB-RIS01-00-SIOENG000</t>
+  </si>
+  <si>
+    <t>OL000081</t>
+  </si>
+  <si>
+    <t>OL000082</t>
   </si>
 </sst>
 </file>
@@ -1377,32 +1383,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L1"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.44140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="8.77734375" style="4"/>
+    <col min="8" max="8" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>0</v>
@@ -1438,12 +1442,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>47</v>
@@ -1457,18 +1461,20 @@
       <c r="F2" s="12">
         <v>0.84652777777777777</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="7">
+        <v>42353</v>
+      </c>
       <c r="H2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="J2" s="28">
         <v>4932</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="11">
@@ -1480,12 +1486,12 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -1502,29 +1508,29 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:XFD94"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.77734375" style="2"/>
+    <col min="8" max="8" width="27.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="23" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="23" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>1</v>
@@ -1533,7 +1539,7 @@
         <v>41</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="F1" s="22" t="s">
         <v>2</v>
@@ -1548,12 +1554,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>47</v>
@@ -1562,7 +1568,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F2" s="13">
         <v>1217</v>
@@ -1580,12 +1586,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>47</v>
@@ -1594,7 +1600,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F3" s="13">
         <v>1217</v>
@@ -1609,12 +1615,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>47</v>
@@ -1623,7 +1629,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F4" s="13">
         <v>1217</v>
@@ -1635,12 +1641,12 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>47</v>
@@ -1649,7 +1655,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F5" s="13">
         <v>1217</v>
@@ -1661,12 +1667,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>47</v>
@@ -1675,7 +1681,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F6" s="13">
         <v>1217</v>
@@ -1687,12 +1693,12 @@
         <v>9.0899999999999995E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>47</v>
@@ -1701,7 +1707,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F7" s="13">
         <v>1217</v>
@@ -1713,12 +1719,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>47</v>
@@ -1727,7 +1733,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F8" s="13">
         <v>1217</v>
@@ -1742,12 +1748,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>47</v>
@@ -1756,7 +1762,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F9" s="13">
         <v>1217</v>
@@ -1771,12 +1777,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>47</v>
@@ -1785,7 +1791,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F10" s="13">
         <v>1217</v>
@@ -1800,12 +1806,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>47</v>
@@ -1814,7 +1820,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F11" s="13">
         <v>1217</v>
@@ -1829,7 +1835,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12"/>
       <c r="C12" s="14"/>
@@ -1838,12 +1844,12 @@
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>47</v>
@@ -1852,10 +1858,10 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>18</v>
@@ -1870,12 +1876,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>47</v>
@@ -1884,10 +1890,10 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>19</v>
@@ -1896,12 +1902,12 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>47</v>
@@ -1910,10 +1916,10 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>20</v>
@@ -1922,12 +1928,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>47</v>
@@ -1936,10 +1942,10 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>21</v>
@@ -1948,12 +1954,12 @@
         <v>38502</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>47</v>
@@ -1962,10 +1968,10 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>22</v>
@@ -1974,12 +1980,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>47</v>
@@ -1988,10 +1994,10 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>23</v>
@@ -2000,12 +2006,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>47</v>
@@ -2014,10 +2020,10 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>39</v>
@@ -2029,7 +2035,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20"/>
       <c r="C20" s="14"/>
@@ -2038,12 +2044,12 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>47</v>
@@ -2052,7 +2058,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F21" s="13">
         <v>392</v>
@@ -2070,12 +2076,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>47</v>
@@ -2084,7 +2090,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F22" s="13">
         <v>392</v>
@@ -2099,12 +2105,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>47</v>
@@ -2113,7 +2119,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F23" s="13">
         <v>392</v>
@@ -2122,10 +2128,10 @@
         <v>15</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24"/>
       <c r="C24" s="14"/>
@@ -2134,12 +2140,12 @@
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>47</v>
@@ -2148,7 +2154,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F25" s="13">
         <v>13992</v>
@@ -2166,12 +2172,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>47</v>
@@ -2180,7 +2186,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F26" s="13">
         <v>13992</v>
@@ -2192,12 +2198,12 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>47</v>
@@ -2206,7 +2212,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F27" s="13">
         <v>13992</v>
@@ -2218,12 +2224,12 @@
         <v>-54.080300000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>47</v>
@@ -2232,7 +2238,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F28" s="13">
         <v>13992</v>
@@ -2244,12 +2250,12 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>47</v>
@@ -2258,7 +2264,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F29" s="13">
         <v>13992</v>
@@ -2270,12 +2276,12 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>47</v>
@@ -2284,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F30" s="13">
         <v>13992</v>
@@ -2296,12 +2302,12 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>47</v>
@@ -2310,7 +2316,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F31" s="13">
         <v>13992</v>
@@ -2322,12 +2328,12 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>47</v>
@@ -2336,7 +2342,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F32" s="13">
         <v>13992</v>
@@ -2348,12 +2354,12 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>47</v>
@@ -2362,7 +2368,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F33" s="13">
         <v>13992</v>
@@ -2374,7 +2380,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34"/>
       <c r="C34" s="14"/>
@@ -2383,12 +2389,12 @@
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
     </row>
-    <row r="35" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>47</v>
@@ -2397,10 +2403,10 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>5</v>
@@ -2415,12 +2421,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>47</v>
@@ -2429,10 +2435,10 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>6</v>
@@ -2441,12 +2447,12 @@
         <v>-54.080300000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>47</v>
@@ -2455,10 +2461,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>7</v>
@@ -2467,12 +2473,12 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>47</v>
@@ -2481,10 +2487,10 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>29</v>
@@ -2493,7 +2499,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39"/>
       <c r="C39" s="14"/>
@@ -2503,12 +2509,12 @@
       <c r="G39" s="13"/>
       <c r="H39" s="26"/>
     </row>
-    <row r="40" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>47</v>
@@ -2517,10 +2523,10 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G40" s="13" t="s">
         <v>5</v>
@@ -2535,12 +2541,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>47</v>
@@ -2549,10 +2555,10 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G41" s="13" t="s">
         <v>6</v>
@@ -2561,12 +2567,12 @@
         <v>-54.080300000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>47</v>
@@ -2575,10 +2581,10 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G42" s="13" t="s">
         <v>7</v>
@@ -2587,12 +2593,12 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>47</v>
@@ -2601,10 +2607,10 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>29</v>
@@ -2613,7 +2619,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44"/>
       <c r="C44" s="14"/>
@@ -2623,12 +2629,12 @@
       <c r="G44" s="13"/>
       <c r="H44" s="26"/>
     </row>
-    <row r="45" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>47</v>
@@ -2637,10 +2643,10 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="G45" s="13" t="s">
         <v>5</v>
@@ -2655,12 +2661,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>47</v>
@@ -2669,10 +2675,10 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="G46" s="13" t="s">
         <v>6</v>
@@ -2681,12 +2687,12 @@
         <v>-54.080300000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>47</v>
@@ -2695,10 +2701,10 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="G47" s="13" t="s">
         <v>7</v>
@@ -2707,12 +2713,12 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>47</v>
@@ -2721,10 +2727,10 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>29</v>
@@ -2733,7 +2739,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49"/>
       <c r="C49" s="14"/>
@@ -2743,12 +2749,12 @@
       <c r="G49" s="13"/>
       <c r="H49" s="26"/>
     </row>
-    <row r="50" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C50" s="14" t="s">
         <v>47</v>
@@ -2757,10 +2763,10 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>5</v>
@@ -2775,12 +2781,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="B51" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C51" s="14" t="s">
         <v>47</v>
@@ -2789,10 +2795,10 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>6</v>
@@ -2801,12 +2807,12 @@
         <v>-54.080300000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>47</v>
@@ -2815,10 +2821,10 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="G52" s="13" t="s">
         <v>7</v>
@@ -2827,12 +2833,12 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="B53" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C53" s="14" t="s">
         <v>47</v>
@@ -2841,10 +2847,10 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="G53" s="13" t="s">
         <v>29</v>
@@ -2853,7 +2859,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54"/>
       <c r="C54" s="14"/>
@@ -2863,12 +2869,12 @@
       <c r="G54" s="13"/>
       <c r="H54" s="26"/>
     </row>
-    <row r="55" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="B55" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C55" s="14" t="s">
         <v>47</v>
@@ -2877,10 +2883,10 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="G55" s="13" t="s">
         <v>5</v>
@@ -2895,12 +2901,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="B56" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>47</v>
@@ -2909,10 +2915,10 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="G56" s="13" t="s">
         <v>6</v>
@@ -2921,12 +2927,12 @@
         <v>-54.080300000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="B57" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C57" s="14" t="s">
         <v>47</v>
@@ -2935,10 +2941,10 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="G57" s="13" t="s">
         <v>7</v>
@@ -2947,12 +2953,12 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>47</v>
@@ -2961,10 +2967,10 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="G58" s="13" t="s">
         <v>29</v>
@@ -2973,7 +2979,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59"/>
       <c r="C59" s="14"/>
@@ -2983,12 +2989,12 @@
       <c r="G59" s="13"/>
       <c r="H59" s="26"/>
     </row>
-    <row r="60" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="B60" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>47</v>
@@ -2997,10 +3003,10 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>5</v>
@@ -3015,12 +3021,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="B61" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>47</v>
@@ -3029,10 +3035,10 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>6</v>
@@ -3041,12 +3047,12 @@
         <v>-54.080300000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>47</v>
@@ -3055,10 +3061,10 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>7</v>
@@ -3067,12 +3073,12 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="B63" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C63" s="14" t="s">
         <v>47</v>
@@ -3081,10 +3087,10 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>29</v>
@@ -3093,7 +3099,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64"/>
       <c r="C64" s="14"/>
@@ -3103,12 +3109,12 @@
       <c r="G64" s="13"/>
       <c r="H64" s="26"/>
     </row>
-    <row r="65" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="B65" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C65" s="14" t="s">
         <v>47</v>
@@ -3117,10 +3123,10 @@
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>5</v>
@@ -3135,12 +3141,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="B66" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C66" s="14" t="s">
         <v>47</v>
@@ -3149,10 +3155,10 @@
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>6</v>
@@ -3161,12 +3167,12 @@
         <v>-54.080300000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="B67" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>47</v>
@@ -3175,10 +3181,10 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="F67" s="24" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>7</v>
@@ -3187,12 +3193,12 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="B68" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>47</v>
@@ -3201,10 +3207,10 @@
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="F68" s="24" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>29</v>
@@ -3213,7 +3219,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69"/>
       <c r="C69" s="14"/>
@@ -3223,12 +3229,12 @@
       <c r="G69" s="13"/>
       <c r="H69" s="26"/>
     </row>
-    <row r="70" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="B70" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>47</v>
@@ -3237,10 +3243,10 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>5</v>
@@ -3255,12 +3261,12 @@
         <v>350</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="B71" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>47</v>
@@ -3269,10 +3275,10 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F71" s="24" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>6</v>
@@ -3281,12 +3287,12 @@
         <v>-54.080300000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="B72" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C72" s="14" t="s">
         <v>47</v>
@@ -3295,10 +3301,10 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>7</v>
@@ -3307,12 +3313,12 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="B73" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>47</v>
@@ -3321,10 +3327,10 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F73" s="24" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>29</v>
@@ -3333,7 +3339,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
       <c r="B74"/>
       <c r="C74" s="14"/>
@@ -3343,12 +3349,12 @@
       <c r="G74" s="13"/>
       <c r="H74" s="26"/>
     </row>
-    <row r="75" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="B75" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>47</v>
@@ -3357,10 +3363,10 @@
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="F75" s="24" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="G75" s="13" t="s">
         <v>5</v>
@@ -3375,12 +3381,12 @@
         <v>501</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="B76" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C76" s="14" t="s">
         <v>47</v>
@@ -3389,10 +3395,10 @@
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="F76" s="24" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="G76" s="13" t="s">
         <v>6</v>
@@ -3401,12 +3407,12 @@
         <v>-54.080300000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="B77" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C77" s="14" t="s">
         <v>47</v>
@@ -3415,10 +3421,10 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="G77" s="13" t="s">
         <v>7</v>
@@ -3427,12 +3433,12 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="B78" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>47</v>
@@ -3441,10 +3447,10 @@
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="F78" s="24" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>29</v>
@@ -3453,7 +3459,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="13"/>
       <c r="B79"/>
       <c r="C79" s="14"/>
@@ -3463,24 +3469,24 @@
       <c r="G79" s="13"/>
       <c r="H79" s="26"/>
     </row>
-    <row r="80" spans="1:10" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="B80" t="s">
+        <v>74</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D80" s="16">
+        <v>1</v>
+      </c>
+      <c r="E80" t="s">
         <v>88</v>
       </c>
-      <c r="C80" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D80" s="16">
-        <v>1</v>
-      </c>
-      <c r="E80" t="s">
-        <v>102</v>
-      </c>
       <c r="F80" s="25" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="G80" s="16" t="s">
         <v>5</v>
@@ -3495,24 +3501,24 @@
         <v>748</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="B81" t="s">
+        <v>74</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D81" s="13">
+        <v>1</v>
+      </c>
+      <c r="E81" t="s">
         <v>88</v>
       </c>
-      <c r="C81" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D81" s="13">
-        <v>1</v>
-      </c>
-      <c r="E81" t="s">
-        <v>102</v>
-      </c>
       <c r="F81" s="24" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="G81" s="13" t="s">
         <v>6</v>
@@ -3521,24 +3527,24 @@
         <v>-54.080300000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="B82" t="s">
+        <v>74</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D82" s="13">
+        <v>1</v>
+      </c>
+      <c r="E82" t="s">
         <v>88</v>
       </c>
-      <c r="C82" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D82" s="13">
-        <v>1</v>
-      </c>
-      <c r="E82" t="s">
-        <v>102</v>
-      </c>
       <c r="F82" s="24" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="G82" s="13" t="s">
         <v>7</v>
@@ -3547,24 +3553,24 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="B83" t="s">
+        <v>74</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D83" s="13">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
         <v>88</v>
       </c>
-      <c r="C83" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D83" s="13">
-        <v>1</v>
-      </c>
-      <c r="E83" t="s">
-        <v>102</v>
-      </c>
       <c r="F83" s="24" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="G83" s="13" t="s">
         <v>29</v>
@@ -3573,7 +3579,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="13"/>
       <c r="B84"/>
       <c r="C84" s="14"/>
@@ -3583,12 +3589,12 @@
       <c r="G84" s="13"/>
       <c r="H84" s="26"/>
     </row>
-    <row r="85" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="B85" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C85" s="14" t="s">
         <v>47</v>
@@ -3597,10 +3603,10 @@
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="F85" s="24" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="G85" s="13" t="s">
         <v>5</v>
@@ -3615,12 +3621,12 @@
         <v>999</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="B86" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C86" s="14" t="s">
         <v>47</v>
@@ -3629,10 +3635,10 @@
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="F86" s="24" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>6</v>
@@ -3641,12 +3647,12 @@
         <v>-54.080300000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="B87" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C87" s="14" t="s">
         <v>47</v>
@@ -3655,10 +3661,10 @@
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="F87" s="24" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>7</v>
@@ -3667,12 +3673,12 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>47</v>
@@ -3681,10 +3687,10 @@
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="F88" s="24" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>29</v>
@@ -3693,7 +3699,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="13"/>
       <c r="B89"/>
       <c r="C89" s="14"/>
@@ -3703,12 +3709,12 @@
       <c r="G89" s="13"/>
       <c r="H89" s="26"/>
     </row>
-    <row r="90" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="B90" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C90" s="14" t="s">
         <v>47</v>
@@ -3717,10 +3723,10 @@
         <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F90" s="24" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>5</v>
@@ -3735,12 +3741,12 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="B91" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C91" s="14" t="s">
         <v>47</v>
@@ -3749,10 +3755,10 @@
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F91" s="24" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>6</v>
@@ -3761,12 +3767,12 @@
         <v>-54.080300000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="B92" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C92" s="14" t="s">
         <v>47</v>
@@ -3775,10 +3781,10 @@
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F92" s="24" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>7</v>
@@ -3787,12 +3793,12 @@
         <v>-88.934600000000003</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="B93" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C93" s="14" t="s">
         <v>47</v>
@@ -3801,10 +3807,10 @@
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F93" s="24" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>29</v>
@@ -3813,7 +3819,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
       <c r="B94"/>
       <c r="C94" s="14"/>
@@ -3823,12 +3829,12 @@
       <c r="G94" s="13"/>
       <c r="H94" s="26"/>
     </row>
-    <row r="95" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A95" s="13" t="s">
-        <v>50</v>
+    <row r="95" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>103</v>
       </c>
       <c r="B95" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C95" s="14" t="s">
         <v>47</v>
@@ -3836,25 +3842,39 @@
       <c r="D95" s="13">
         <v>1</v>
       </c>
-      <c r="E95" s="13"/>
-      <c r="F95" s="20" t="s">
-        <v>54</v>
+      <c r="E95" t="s">
+        <v>105</v>
+      </c>
+      <c r="F95" s="20">
+        <v>13997</v>
       </c>
       <c r="G95" s="13"/>
       <c r="I95" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A96" s="13"/>
-      <c r="B96" s="13"/>
-      <c r="C96" s="14"/>
-      <c r="D96" s="13"/>
-      <c r="E96" s="13"/>
-      <c r="F96" s="13"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>104</v>
+      </c>
+      <c r="B96" t="s">
+        <v>74</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D96" s="13">
+        <v>1</v>
+      </c>
+      <c r="E96" t="s">
+        <v>106</v>
+      </c>
+      <c r="F96" s="13">
+        <v>13991</v>
+      </c>
       <c r="G96" s="13"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
       <c r="B97" s="13"/>
       <c r="C97" s="13"/>
@@ -3863,7 +3883,7 @@
       <c r="F97" s="13"/>
       <c r="G97" s="13"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="13"/>
       <c r="B98" s="13"/>
       <c r="C98" s="13"/>
@@ -3872,7 +3892,7 @@
       <c r="F98" s="13"/>
       <c r="G98" s="13"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="13"/>
       <c r="B99" s="13"/>
       <c r="C99" s="13"/>
@@ -3881,7 +3901,7 @@
       <c r="F99" s="13"/>
       <c r="G99" s="13"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="13"/>
       <c r="B100" s="13"/>
       <c r="C100" s="13"/>
@@ -3890,7 +3910,7 @@
       <c r="F100" s="13"/>
       <c r="G100" s="13"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
       <c r="B101" s="13"/>
       <c r="C101" s="13"/>

</xml_diff>